<commit_message>
add back a few soldermask gaps
</commit_message>
<xml_diff>
--- a/hardware/kicad/production/OO_TrafficPCB_V2_0_BOM_pcbway.xlsx
+++ b/hardware/kicad/production/OO_TrafficPCB_V2_0_BOM_pcbway.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28429"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bapti\Documents\traffic-pcb-sb\hardware\kicad\jlcpcb\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bapti\Documents\traffic-pcb-sb\hardware\kicad\production\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D997A3CF-4D89-403E-8DE2-73C2B394782F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8E96818-D288-41FB-B456-73E47BB92971}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="20430" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -153,9 +153,6 @@
     <t>LED_RGB_0606</t>
   </si>
   <si>
-    <t>R100,R101,R103,R104,R110,R111,R113,R114,R117,R118,R12,R120,R121,R123,R124,R126,R127,R129,R13,R130,R132,R133,R135,R136,R138,R139,R145,R146,R147,R148,R149,R15,R150,R151,R152,R153,R154,R155,R156,R157,R158,R159,R16,R160,R161,R162,R163,R164,R165,R166,R167,R168,R169,R170,R171,R172,R173,R174,R175,R176,R177,R178,R179,R180,R181,R182,R183,R184,R185,R186,R187,R188,R22,R23,R25,R26,R29,R30,R32,R33,R35,R36,R38,R39,R41,R42,R44,R45,R47,R48,R50,R51,R53,R54,R56,R57,R59,R60,R66,R67,R69,R70,R73,R74,R76,R77,R79,R80,R82,R83,R85,R86,R88,R89,R91,R92,R94,R95,R97,R98</t>
-  </si>
-  <si>
     <t>YAGEO</t>
   </si>
   <si>
@@ -231,9 +228,6 @@
     <t>QFN40P700X700X80-61N</t>
   </si>
   <si>
-    <t>R115,R27,R71</t>
-  </si>
-  <si>
     <t>LCSC: C25804</t>
   </si>
   <si>
@@ -565,6 +559,12 @@
   </si>
   <si>
     <t>LCSC: C2913198 (N4,N8, or any other ok)</t>
+  </si>
+  <si>
+    <t>R100,R101,R103,R104,R110,R111,R113,R114,R117,R118,R12,R120,R121,R123,R124,R126,R127,R129,R13,R130,R132,R133,R135,R136,R138,R139,R145,R146,R147,R148,R15,R150,R151,R152,R153,R154,R155,R156,R157,R158,R159,R16,R160,R161,R162,R163,R164,R165,R166,R167,R168,R169,R170,R171,R172,R173,R174,R175,R176,R177,R178,R179,R180,R181,R182,R183,R184,R185,R186,R187,R188,R22,R23,R25,R26,R29,R30,R32,R33,R35,R36,R38,R39,R41,R42,R44,R45,R47,R48,R50,R51,R53,R54,R56,R57,R59,R60,R66,R67,R69,R70,R73,R74,R76,R77,R79,R80,R82,R83,R85,R86,R88,R89,R91,R92,R94,R95,R97,R98</t>
+  </si>
+  <si>
+    <t>R115,R27,R71,R149</t>
   </si>
 </sst>
 </file>
@@ -1079,7 +1079,7 @@
   <dimension ref="A2:I34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L43" sqref="L43"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
@@ -1100,7 +1100,7 @@
       <c r="A2" s="14"/>
       <c r="B2" s="14"/>
       <c r="D2" s="12" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="E2" s="13"/>
       <c r="F2" s="13"/>
@@ -1151,7 +1151,7 @@
         <v>1</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C7" s="6">
         <v>413</v>
@@ -1172,7 +1172,7 @@
         <v>9</v>
       </c>
       <c r="I7" s="9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="15.75">
@@ -1201,7 +1201,7 @@
         <v>9</v>
       </c>
       <c r="I8" s="10" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="15.75">
@@ -1209,19 +1209,19 @@
         <v>3</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>19</v>
+        <v>155</v>
       </c>
       <c r="C9" s="6">
         <v>120</v>
       </c>
       <c r="D9" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="E9" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="E9" s="7" t="s">
+      <c r="F9" s="8" t="s">
         <v>21</v>
-      </c>
-      <c r="F9" s="8" t="s">
-        <v>22</v>
       </c>
       <c r="G9" s="10" t="s">
         <v>17</v>
@@ -1230,7 +1230,7 @@
         <v>9</v>
       </c>
       <c r="I9" s="9" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="15.75">
@@ -1238,28 +1238,28 @@
         <v>4</v>
       </c>
       <c r="B10" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" s="6">
+        <v>9</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="F10" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="G10" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="C10" s="6">
-        <v>9</v>
-      </c>
-      <c r="D10" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="E10" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="F10" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="G10" s="10" t="s">
+      <c r="H10" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="I10" s="9" t="s">
         <v>25</v>
-      </c>
-      <c r="H10" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="I10" s="9" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="15.75">
@@ -1267,28 +1267,28 @@
         <v>5</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C11" s="6">
         <v>12</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E11" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="F11" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="F11" s="8" t="s">
-        <v>33</v>
-      </c>
       <c r="G11" s="10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H11" s="9" t="s">
         <v>9</v>
       </c>
       <c r="I11" s="9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="15.75">
@@ -1296,19 +1296,19 @@
         <v>6</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C12" s="6">
         <v>6</v>
       </c>
       <c r="D12" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="E12" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="E12" s="7" t="s">
+      <c r="F12" s="8" t="s">
         <v>37</v>
-      </c>
-      <c r="F12" s="8" t="s">
-        <v>38</v>
       </c>
       <c r="G12" s="10" t="s">
         <v>17</v>
@@ -1317,7 +1317,7 @@
         <v>9</v>
       </c>
       <c r="I12" s="9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="15.75">
@@ -1325,28 +1325,28 @@
         <v>7</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C13" s="6">
         <v>4</v>
       </c>
       <c r="D13" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="F13" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="E13" s="7" t="s">
+      <c r="G13" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="F13" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="G13" s="10" t="s">
-        <v>44</v>
-      </c>
       <c r="H13" s="9" t="s">
         <v>9</v>
       </c>
       <c r="I13" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="15.75">
@@ -1354,28 +1354,28 @@
         <v>8</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>45</v>
+        <v>156</v>
       </c>
       <c r="C14" s="6">
         <v>3</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E14" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="F14" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="G14" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="F14" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="G14" s="10" t="s">
-        <v>49</v>
-      </c>
       <c r="H14" s="9" t="s">
         <v>9</v>
       </c>
       <c r="I14" s="9" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="15.75">
@@ -1383,28 +1383,28 @@
         <v>9</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C15" s="6">
         <v>3</v>
       </c>
       <c r="D15" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="F15" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="E15" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="F15" s="7" t="s">
-        <v>56</v>
-      </c>
       <c r="G15" s="10" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="H15" s="9" t="s">
         <v>9</v>
       </c>
       <c r="I15" s="9" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="15.75">
@@ -1412,19 +1412,19 @@
         <v>10</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C16" s="6">
         <v>3</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F16" s="7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="G16" s="10" t="s">
         <v>17</v>
@@ -1433,7 +1433,7 @@
         <v>9</v>
       </c>
       <c r="I16" s="10" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="15.75">
@@ -1441,28 +1441,28 @@
         <v>11</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C17" s="6">
         <v>2</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F17" s="7" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="G17" s="10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H17" s="9" t="s">
         <v>9</v>
       </c>
       <c r="I17" s="9" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="15.75">
@@ -1470,28 +1470,28 @@
         <v>12</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C18" s="6">
         <v>2</v>
       </c>
       <c r="D18" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="E18" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="F18" s="8" t="s">
         <v>126</v>
       </c>
-      <c r="E18" s="7" t="s">
+      <c r="G18" s="10" t="s">
+        <v>123</v>
+      </c>
+      <c r="H18" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="I18" s="9" t="s">
         <v>127</v>
-      </c>
-      <c r="F18" s="8" t="s">
-        <v>128</v>
-      </c>
-      <c r="G18" s="10" t="s">
-        <v>125</v>
-      </c>
-      <c r="H18" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="I18" s="9" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="15.75">
@@ -1499,28 +1499,28 @@
         <v>13</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C19" s="6">
         <v>2</v>
       </c>
       <c r="D19" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="E19" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="F19" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="E19" s="7" t="s">
+      <c r="G19" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="F19" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="G19" s="10" t="s">
-        <v>72</v>
-      </c>
       <c r="H19" s="9" t="s">
         <v>9</v>
       </c>
       <c r="I19" s="9" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="15.75">
@@ -1528,19 +1528,19 @@
         <v>14</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C20" s="6">
         <v>2</v>
       </c>
       <c r="D20" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E20" s="7" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F20" s="7" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="G20" s="10" t="s">
         <v>17</v>
@@ -1549,7 +1549,7 @@
         <v>9</v>
       </c>
       <c r="I20" s="9" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="15.75">
@@ -1557,19 +1557,19 @@
         <v>15</v>
       </c>
       <c r="B21" s="10" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C21" s="6">
         <v>2</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E21" s="7" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="F21" s="8" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G21" s="10" t="s">
         <v>17</v>
@@ -1578,7 +1578,7 @@
         <v>9</v>
       </c>
       <c r="I21" s="9" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="22" spans="1:9" ht="15.75">
@@ -1586,28 +1586,28 @@
         <v>16</v>
       </c>
       <c r="B22" s="10" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C22" s="6">
         <v>2</v>
       </c>
       <c r="D22" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="E22" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="F22" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="E22" s="7" t="s">
-        <v>85</v>
-      </c>
-      <c r="F22" s="8" t="s">
-        <v>86</v>
-      </c>
       <c r="G22" s="10" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="H22" s="9" t="s">
         <v>9</v>
       </c>
       <c r="I22" s="9" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="23" spans="1:9" ht="15.75">
@@ -1615,19 +1615,19 @@
         <v>17</v>
       </c>
       <c r="B23" s="10" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C23" s="6">
         <v>1</v>
       </c>
       <c r="D23" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E23" s="7" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="F23" s="8" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="G23" s="10" t="s">
         <v>17</v>
@@ -1636,7 +1636,7 @@
         <v>9</v>
       </c>
       <c r="I23" s="9" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="24" spans="1:9" ht="15.75">
@@ -1644,28 +1644,28 @@
         <v>20</v>
       </c>
       <c r="B24" s="10" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C24" s="6">
         <v>1</v>
       </c>
       <c r="D24" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E24" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="F24" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="G24" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="F24" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="G24" s="10" t="s">
-        <v>95</v>
-      </c>
       <c r="H24" s="9" t="s">
         <v>9</v>
       </c>
       <c r="I24" s="9" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="25" spans="1:9" ht="15.75">
@@ -1673,28 +1673,28 @@
         <v>21</v>
       </c>
       <c r="B25" s="10" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C25" s="6">
         <v>1</v>
       </c>
       <c r="D25" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="E25" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="F25" s="8" t="s">
         <v>97</v>
       </c>
-      <c r="E25" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="F25" s="8" t="s">
-        <v>99</v>
-      </c>
       <c r="G25" s="10" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="H25" s="9" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="I25" s="9" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="26" spans="1:9" ht="15.75">
@@ -1702,28 +1702,28 @@
         <v>22</v>
       </c>
       <c r="B26" s="10" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C26" s="6">
         <v>1</v>
       </c>
       <c r="D26" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="E26" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="F26" s="8" t="s">
         <v>105</v>
       </c>
-      <c r="E26" s="7" t="s">
-        <v>106</v>
-      </c>
-      <c r="F26" s="8" t="s">
-        <v>107</v>
-      </c>
       <c r="G26" s="10" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="H26" s="9" t="s">
         <v>9</v>
       </c>
       <c r="I26" s="9" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="27" spans="1:9" ht="15.75">
@@ -1731,28 +1731,28 @@
         <v>23</v>
       </c>
       <c r="B27" s="10" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C27" s="6">
         <v>1</v>
       </c>
       <c r="D27" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="E27" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="F27" s="8" t="s">
         <v>110</v>
       </c>
-      <c r="E27" s="7" t="s">
+      <c r="G27" s="10" t="s">
         <v>111</v>
       </c>
-      <c r="F27" s="8" t="s">
-        <v>112</v>
-      </c>
-      <c r="G27" s="10" t="s">
-        <v>113</v>
-      </c>
       <c r="H27" s="9" t="s">
         <v>9</v>
       </c>
       <c r="I27" s="9" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="28" spans="1:9" ht="15.75">
@@ -1760,28 +1760,28 @@
         <v>24</v>
       </c>
       <c r="B28" s="10" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C28" s="6">
         <v>1</v>
       </c>
       <c r="D28" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="E28" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="F28" s="8" t="s">
         <v>115</v>
       </c>
-      <c r="E28" s="7" t="s">
+      <c r="G28" s="10" t="s">
         <v>116</v>
       </c>
-      <c r="F28" s="8" t="s">
-        <v>117</v>
-      </c>
-      <c r="G28" s="10" t="s">
-        <v>118</v>
-      </c>
       <c r="H28" s="9" t="s">
         <v>9</v>
       </c>
       <c r="I28" s="9" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="29" spans="1:9" ht="15.75">
@@ -1789,28 +1789,28 @@
         <v>25</v>
       </c>
       <c r="B29" s="10" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C29" s="6">
         <v>1</v>
       </c>
       <c r="D29" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="E29" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="F29" s="8" t="s">
         <v>132</v>
       </c>
-      <c r="E29" s="7" t="s">
+      <c r="G29" s="10" t="s">
         <v>133</v>
       </c>
-      <c r="F29" s="8" t="s">
-        <v>134</v>
-      </c>
-      <c r="G29" s="10" t="s">
-        <v>135</v>
-      </c>
       <c r="H29" s="9" t="s">
         <v>9</v>
       </c>
       <c r="I29" s="9" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="30" spans="1:9" ht="15.75">
@@ -1818,28 +1818,28 @@
         <v>26</v>
       </c>
       <c r="B30" s="10" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C30" s="6">
         <v>1</v>
       </c>
       <c r="D30" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E30" s="7" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="F30" s="8" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="G30" s="10" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="H30" s="9" t="s">
         <v>9</v>
       </c>
       <c r="I30" s="9" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="31" spans="1:9" ht="16.5" customHeight="1">
@@ -1847,28 +1847,28 @@
         <v>27</v>
       </c>
       <c r="B31" s="10" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C31" s="6">
         <v>1</v>
       </c>
       <c r="D31" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E31" s="11" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="F31" s="8" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="G31" s="10" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="H31" s="9" t="s">
         <v>9</v>
       </c>
       <c r="I31" s="9" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="32" spans="1:9" ht="15.75">
@@ -1876,28 +1876,28 @@
         <v>28</v>
       </c>
       <c r="B32" s="10" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C32" s="6">
         <v>1</v>
       </c>
       <c r="D32" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E32" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="F32" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="G32" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="H32" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="I32" s="9" t="s">
         <v>145</v>
-      </c>
-      <c r="F32" s="8" t="s">
-        <v>146</v>
-      </c>
-      <c r="G32" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="H32" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="I32" s="9" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="33" spans="1:9" ht="15.75">
@@ -1905,28 +1905,28 @@
         <v>29</v>
       </c>
       <c r="B33" s="10" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C33" s="6">
         <v>1</v>
       </c>
       <c r="D33" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E33" s="7" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F33" s="8" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="G33" s="10" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="H33" s="9" t="s">
         <v>9</v>
       </c>
       <c r="I33" s="9" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="34" spans="1:9" ht="15.75">
@@ -1934,28 +1934,28 @@
         <v>25</v>
       </c>
       <c r="B34" s="10" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C34" s="6">
         <v>1</v>
       </c>
       <c r="D34" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="E34" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="F34" s="8" t="s">
         <v>120</v>
       </c>
-      <c r="E34" s="7" t="s">
+      <c r="G34" s="9" t="s">
         <v>121</v>
       </c>
-      <c r="F34" s="8" t="s">
+      <c r="H34" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="I34" s="9" t="s">
         <v>122</v>
-      </c>
-      <c r="G34" s="9" t="s">
-        <v>123</v>
-      </c>
-      <c r="H34" s="9" t="s">
-        <v>153</v>
-      </c>
-      <c r="I34" s="9" t="s">
-        <v>124</v>
       </c>
     </row>
   </sheetData>

</xml_diff>